<commit_message>
Fixed some issues with v0.4 (SMD)
</commit_message>
<xml_diff>
--- a/v0.4/SMD/Latest/v0.4.4c BOM.xlsx
+++ b/v0.4/SMD/Latest/v0.4.4c BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/Speeduino-Boards-Private/v0.4/0.4.4c/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Documents\Git\Speeduino\v0.4\SMD\Latest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D12D5F7A-705D-CB41-AA23-A428B011B37F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B88AD7-F215-407F-82C3-663836AE3458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="520" windowWidth="26840" windowHeight="14560"/>
+    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v0.4.4c" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="206">
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Quantity</t>
   </si>
   <si>
@@ -34,12 +31,6 @@
     <t xml:space="preserve"> Footprint</t>
   </si>
   <si>
-    <t xml:space="preserve"> Manufacturer_Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Manufacturer_Part_Number</t>
-  </si>
-  <si>
     <t xml:space="preserve"> URL</t>
   </si>
   <si>
@@ -638,12 +629,21 @@
   </si>
   <si>
     <t>Pins on underside of board</t>
+  </si>
+  <si>
+    <t>Designator</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Mfr. Part #</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1491,975 +1491,975 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.83203125" customWidth="1"/>
+    <col min="1" max="1" width="65.875" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="66.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
-    <col min="6" max="6" width="33.83203125" customWidth="1"/>
-    <col min="7" max="7" width="103.33203125" customWidth="1"/>
+    <col min="4" max="4" width="66.375" customWidth="1"/>
+    <col min="5" max="5" width="18.875" customWidth="1"/>
+    <col min="6" max="6" width="33.875" customWidth="1"/>
+    <col min="7" max="7" width="103.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>203</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>204</v>
+      </c>
+      <c r="F1" t="s">
+        <v>205</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>13</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" t="s">
+      <c r="G3" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>16</v>
-      </c>
-      <c r="F3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>19</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="G4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>25</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G5" t="s">
         <v>27</v>
       </c>
-      <c r="E5" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>28</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>31</v>
       </c>
       <c r="B6">
         <v>13</v>
       </c>
       <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>35</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>36</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>39</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
       <c r="C8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>43</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>44</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>45</v>
-      </c>
-      <c r="G9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>47</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
       <c r="C10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s">
         <v>48</v>
       </c>
-      <c r="D10" t="s">
+      <c r="G10" t="s">
         <v>49</v>
       </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>50</v>
-      </c>
-      <c r="F10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>53</v>
       </c>
       <c r="B11">
         <v>2</v>
       </c>
       <c r="C11" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" t="s">
         <v>54</v>
       </c>
-      <c r="D11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>55</v>
-      </c>
-      <c r="F11" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>58</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>60</v>
-      </c>
-      <c r="E12" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>63</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>64</v>
-      </c>
-      <c r="D13" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>67</v>
       </c>
       <c r="B14">
         <v>8</v>
       </c>
       <c r="C14" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" t="s">
         <v>68</v>
       </c>
-      <c r="D14" t="s">
+      <c r="G14" t="s">
         <v>69</v>
       </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>70</v>
-      </c>
-      <c r="F14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>73</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" t="s">
         <v>74</v>
       </c>
-      <c r="D15" t="s">
+      <c r="G15" t="s">
         <v>75</v>
       </c>
-      <c r="E15" t="s">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>76</v>
-      </c>
-      <c r="F15" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>79</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F16" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E17" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F17" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F18" t="s">
+        <v>197</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>86</v>
-      </c>
-      <c r="D18" t="s">
-        <v>87</v>
-      </c>
-      <c r="E18" t="s">
-        <v>201</v>
-      </c>
-      <c r="F18" t="s">
-        <v>200</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>89</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E19" t="s">
+        <v>88</v>
+      </c>
+      <c r="F19" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" t="s">
         <v>90</v>
       </c>
-      <c r="D19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>91</v>
-      </c>
-      <c r="F19" t="s">
-        <v>92</v>
-      </c>
-      <c r="G19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>94</v>
       </c>
       <c r="B20">
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D20" t="s">
+        <v>85</v>
+      </c>
+      <c r="E20" t="s">
         <v>88</v>
       </c>
-      <c r="E20" t="s">
-        <v>91</v>
-      </c>
       <c r="F20" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="G20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>96</v>
       </c>
       <c r="B21">
         <v>2</v>
       </c>
       <c r="C21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" t="s">
+        <v>88</v>
+      </c>
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" t="s">
         <v>97</v>
       </c>
-      <c r="D21" t="s">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>98</v>
-      </c>
-      <c r="E21" t="s">
-        <v>91</v>
-      </c>
-      <c r="F21" t="s">
-        <v>99</v>
-      </c>
-      <c r="G21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>101</v>
       </c>
       <c r="B22">
         <v>3</v>
       </c>
       <c r="C22" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" t="s">
+        <v>100</v>
+      </c>
+      <c r="E22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" t="s">
         <v>102</v>
       </c>
-      <c r="D22" t="s">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>103</v>
-      </c>
-      <c r="E22" t="s">
-        <v>104</v>
-      </c>
-      <c r="F22" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>106</v>
       </c>
       <c r="B23">
         <v>12</v>
       </c>
       <c r="C23" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" t="s">
+        <v>105</v>
+      </c>
+      <c r="E23" t="s">
+        <v>7</v>
+      </c>
+      <c r="F23" t="s">
+        <v>106</v>
+      </c>
+      <c r="G23" t="s">
         <v>107</v>
       </c>
-      <c r="D23" t="s">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>108</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>109</v>
-      </c>
-      <c r="G23" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>111</v>
       </c>
       <c r="B24">
         <v>9</v>
       </c>
       <c r="C24" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" t="s">
+        <v>105</v>
+      </c>
+      <c r="E24" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" t="s">
+        <v>110</v>
+      </c>
+      <c r="G24" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>112</v>
-      </c>
-      <c r="D24" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>113</v>
-      </c>
-      <c r="G24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>115</v>
       </c>
       <c r="B25">
         <v>4</v>
       </c>
       <c r="C25" t="s">
+        <v>113</v>
+      </c>
+      <c r="D25" t="s">
+        <v>105</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+      <c r="F25" t="s">
+        <v>114</v>
+      </c>
+      <c r="G25" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>116</v>
-      </c>
-      <c r="D25" t="s">
-        <v>108</v>
-      </c>
-      <c r="E25" t="s">
-        <v>10</v>
-      </c>
-      <c r="F25" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>119</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
+        <v>117</v>
+      </c>
+      <c r="D26" t="s">
+        <v>105</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>120</v>
-      </c>
-      <c r="D26" t="s">
-        <v>108</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
-        <v>121</v>
-      </c>
-      <c r="G26" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>123</v>
       </c>
       <c r="B27">
         <v>9</v>
       </c>
       <c r="C27" t="s">
+        <v>121</v>
+      </c>
+      <c r="D27" t="s">
+        <v>105</v>
+      </c>
+      <c r="E27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F27" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" t="s">
         <v>124</v>
       </c>
-      <c r="D27" t="s">
-        <v>108</v>
-      </c>
-      <c r="E27" t="s">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>125</v>
-      </c>
-      <c r="F27" t="s">
-        <v>126</v>
-      </c>
-      <c r="G27" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>128</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>127</v>
+      </c>
+      <c r="G28" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>129</v>
-      </c>
-      <c r="D28" t="s">
-        <v>108</v>
-      </c>
-      <c r="E28" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28" t="s">
-        <v>130</v>
-      </c>
-      <c r="G28" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>132</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
+        <v>130</v>
+      </c>
+      <c r="D29" t="s">
+        <v>105</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>133</v>
-      </c>
-      <c r="D29" t="s">
-        <v>108</v>
-      </c>
-      <c r="E29" t="s">
-        <v>10</v>
-      </c>
-      <c r="F29" t="s">
-        <v>134</v>
-      </c>
-      <c r="G29" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>136</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" t="s">
+        <v>105</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>137</v>
-      </c>
-      <c r="D30" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" t="s">
-        <v>138</v>
-      </c>
-      <c r="G30" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>140</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D31" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>139</v>
+      </c>
+      <c r="G31" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>141</v>
-      </c>
-      <c r="D31" t="s">
-        <v>108</v>
-      </c>
-      <c r="E31" t="s">
-        <v>10</v>
-      </c>
-      <c r="F31" t="s">
-        <v>142</v>
-      </c>
-      <c r="G31" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>144</v>
       </c>
       <c r="B32">
         <v>18</v>
       </c>
       <c r="C32" t="s">
+        <v>142</v>
+      </c>
+      <c r="D32" t="s">
+        <v>105</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>143</v>
+      </c>
+      <c r="G32" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>145</v>
-      </c>
-      <c r="D32" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" t="s">
-        <v>146</v>
-      </c>
-      <c r="G32" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>148</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" t="s">
+        <v>146</v>
+      </c>
+      <c r="D33" t="s">
+        <v>105</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>147</v>
+      </c>
+      <c r="G33" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>149</v>
-      </c>
-      <c r="D33" t="s">
-        <v>108</v>
-      </c>
-      <c r="E33" t="s">
-        <v>10</v>
-      </c>
-      <c r="F33" t="s">
-        <v>150</v>
-      </c>
-      <c r="G33" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>152</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" t="s">
+        <v>150</v>
+      </c>
+      <c r="D34" t="s">
+        <v>151</v>
+      </c>
+      <c r="E34" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" t="s">
         <v>153</v>
       </c>
-      <c r="D34" t="s">
+      <c r="G34" t="s">
         <v>154</v>
       </c>
-      <c r="E34" t="s">
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>155</v>
-      </c>
-      <c r="F34" t="s">
-        <v>156</v>
-      </c>
-      <c r="G34" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>158</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" t="s">
+        <v>156</v>
+      </c>
+      <c r="D35" t="s">
+        <v>157</v>
+      </c>
+      <c r="E35" t="s">
+        <v>158</v>
+      </c>
+      <c r="F35" t="s">
+        <v>156</v>
+      </c>
+      <c r="G35" t="s">
         <v>159</v>
       </c>
-      <c r="D35" t="s">
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>160</v>
-      </c>
-      <c r="E35" t="s">
-        <v>161</v>
-      </c>
-      <c r="F35" t="s">
-        <v>159</v>
-      </c>
-      <c r="G35" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>163</v>
       </c>
       <c r="B36">
         <v>4</v>
       </c>
       <c r="C36" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" t="s">
+        <v>163</v>
+      </c>
+      <c r="F36" t="s">
         <v>164</v>
       </c>
-      <c r="D36" t="s">
+      <c r="G36" t="s">
         <v>165</v>
       </c>
-      <c r="E36" t="s">
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>166</v>
-      </c>
-      <c r="F36" t="s">
-        <v>167</v>
-      </c>
-      <c r="G36" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>169</v>
       </c>
       <c r="B37">
         <v>2</v>
       </c>
       <c r="C37" t="s">
+        <v>167</v>
+      </c>
+      <c r="D37" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" t="s">
+        <v>168</v>
+      </c>
+      <c r="F37" t="s">
+        <v>169</v>
+      </c>
+      <c r="G37" t="s">
         <v>170</v>
       </c>
-      <c r="D37" t="s">
-        <v>165</v>
-      </c>
-      <c r="E37" t="s">
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>171</v>
-      </c>
-      <c r="F37" t="s">
-        <v>172</v>
-      </c>
-      <c r="G37" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>174</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
+        <v>172</v>
+      </c>
+      <c r="D38" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" t="s">
+        <v>174</v>
+      </c>
+      <c r="F38" t="s">
         <v>175</v>
       </c>
-      <c r="D38" t="s">
+      <c r="G38" t="s">
         <v>176</v>
       </c>
-      <c r="E38" t="s">
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>177</v>
-      </c>
-      <c r="F38" t="s">
-        <v>178</v>
-      </c>
-      <c r="G38" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>180</v>
       </c>
       <c r="B39">
         <v>1</v>
       </c>
       <c r="C39" t="s">
+        <v>178</v>
+      </c>
+      <c r="D39" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" t="s">
         <v>181</v>
       </c>
-      <c r="D39" t="s">
+      <c r="G39" t="s">
         <v>182</v>
       </c>
-      <c r="E39" t="s">
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>183</v>
-      </c>
-      <c r="F39" t="s">
-        <v>184</v>
-      </c>
-      <c r="G39" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>186</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
       <c r="C40" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" t="s">
+        <v>185</v>
+      </c>
+      <c r="E40" t="s">
+        <v>186</v>
+      </c>
+      <c r="F40" t="s">
+        <v>184</v>
+      </c>
+      <c r="G40" t="s">
         <v>187</v>
       </c>
-      <c r="D40" t="s">
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>188</v>
-      </c>
-      <c r="E40" t="s">
-        <v>189</v>
-      </c>
-      <c r="F40" t="s">
-        <v>187</v>
-      </c>
-      <c r="G40" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>191</v>
       </c>
       <c r="B41">
         <v>4</v>
       </c>
       <c r="C41" t="s">
+        <v>189</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="F41" t="s">
         <v>192</v>
       </c>
-      <c r="D41" s="1" t="s">
+      <c r="G41" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="F41" t="s">
-        <v>195</v>
-      </c>
-      <c r="G41" s="2" t="s">
-        <v>196</v>
-      </c>
       <c r="H41" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G41" r:id="rId1"/>
-    <hyperlink ref="G17" r:id="rId2"/>
-    <hyperlink ref="G18" r:id="rId3"/>
-    <hyperlink ref="G16" r:id="rId4"/>
+    <hyperlink ref="G41" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G17" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G18" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G16" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>